<commit_message>
Added new sheet to incorporate sprint 2
</commit_message>
<xml_diff>
--- a/DevelopmentDocuments/ganttCharts.xlsx
+++ b/DevelopmentDocuments/ganttCharts.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b6d8a147596ee6a2/Documents/GitHub/PropertyTycoon/DevelopmentDocuments/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agent\OneDrive\Documents\GitHub\PropertyTycoon\DevelopmentDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="8_{DD5C7697-C4C7-4BC1-A1F4-95C252628761}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{75FE02E4-7E5A-4C53-BC47-C57B7954283C}"/>
+  <xr:revisionPtr revIDLastSave="94" documentId="8_{DD5C7697-C4C7-4BC1-A1F4-95C252628761}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{9B21D3F6-02F7-44D4-A5A0-92D76774FBB1}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{36599407-A2B4-4F4E-B01D-CD4A00EBB384}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{36599407-A2B4-4F4E-B01D-CD4A00EBB384}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sprint2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>Sprint1</t>
   </si>
@@ -65,12 +66,33 @@
   <si>
     <t>Testing</t>
   </si>
+  <si>
+    <t>Sprint 2</t>
+  </si>
+  <si>
+    <t>Rent feature</t>
+  </si>
+  <si>
+    <t>Basic GUI</t>
+  </si>
+  <si>
+    <t>Text-based game</t>
+  </si>
+  <si>
+    <t>Player tokens</t>
+  </si>
+  <si>
+    <t>Possible player actions</t>
+  </si>
+  <si>
+    <t>Update game objects</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,6 +103,14 @@
     <font>
       <b/>
       <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -107,7 +137,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -116,6 +146,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -573,7 +609,461 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-AU"/>
+              <a:t>Sprint 2</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sprint2!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Start Date</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sprint2!$A$3:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Rent feature</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Update game objects</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Basic GUI</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Text-based game</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Possible player actions</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Player tokens</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sprint2!$B$3:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>43871</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43871</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43871</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43872</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43873</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43874</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9D24-4458-B8EE-2C448556C3FF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sprint2!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Duration</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sprint2!$A$3:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Rent feature</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Update game objects</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Basic GUI</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Text-based game</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Possible player actions</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Player tokens</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sprint2!$C$3:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9D24-4458-B8EE-2C448556C3FF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="658045800"/>
+        <c:axId val="694105048"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="658045800"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="694105048"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="694105048"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="43878"/>
+          <c:min val="43871"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="t"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="658045800"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1118,6 +1608,511 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1139,6 +2134,47 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71CC8AF0-1A23-4D7C-8808-6A77EB5639D5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>263525</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>73025</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>568325</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>53975</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB221EC4-BF8D-4A8F-9DCF-3909825422E2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1458,7 +2494,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F91177E-DECF-4A73-9BA7-D4A513C33052}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -1588,4 +2624,114 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56660406-3394-4E0E-884A-71C01CDEF536}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="25.7265625" customWidth="1"/>
+    <col min="2" max="2" width="18.7265625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2">
+        <v>43871</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="2">
+        <v>43871</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="2">
+        <v>43871</v>
+      </c>
+      <c r="C5" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="2">
+        <v>43872</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="2">
+        <v>43873</v>
+      </c>
+      <c r="C7" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="2">
+        <v>43874</v>
+      </c>
+      <c r="C8" s="1">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:C8">
+    <sortCondition ref="B3:B8"/>
+    <sortCondition ref="C3:C8"/>
+  </sortState>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Created gantt chart for sprint 8
</commit_message>
<xml_diff>
--- a/DevelopmentDocuments/ganttCharts.xlsx
+++ b/DevelopmentDocuments/ganttCharts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agent\Desktop\Projects\PropertyTycoon\DevelopmentDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{456AC1BB-644E-44BE-B204-AFB6CAF4902A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7593AC61-5882-47D6-9754-720C058C4FCF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-29595" yWindow="9840" windowWidth="38700" windowHeight="15885" firstSheet="3" activeTab="6" xr2:uid="{36599407-A2B4-4F4E-B01D-CD4A00EBB384}"/>
+    <workbookView xWindow="-31755" yWindow="3840" windowWidth="38700" windowHeight="15885" firstSheet="3" activeTab="7" xr2:uid="{36599407-A2B4-4F4E-B01D-CD4A00EBB384}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="66">
   <si>
     <t>Sprint1</t>
   </si>
@@ -220,6 +220,24 @@
   </si>
   <si>
     <t>update GUI</t>
+  </si>
+  <si>
+    <t>Fix rolling doubles issue</t>
+  </si>
+  <si>
+    <t>Fix doubles jail issue</t>
+  </si>
+  <si>
+    <t>Fix landing on Go issue</t>
+  </si>
+  <si>
+    <t>Stations/Utilities cannot be bought in first loop</t>
+  </si>
+  <si>
+    <t>Animate tokens as gifs in GUI</t>
+  </si>
+  <si>
+    <t>In auction, if all bids 0, cancel auction</t>
   </si>
 </sst>
 </file>
@@ -3252,6 +3270,420 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="728754688"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-CH"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-AU"/>
+              <a:t>Sprint 8</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-CH"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sprint8!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Start Date</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sprint8!$A$3:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Stations/Utilities cannot be bought in first loop</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Fix rolling doubles issue</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Animate tokens as gifs in GUI</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>In auction, if all bids 0, cancel auction</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Fix doubles jail issue</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Fix landing on Go issue</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sprint8!$B$3:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>43934</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43934</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43934</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43935</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43936</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43939</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-15AF-4DD6-AB71-2278BE4BB518}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sprint8!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Duration</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sprint8!$A$3:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Stations/Utilities cannot be bought in first loop</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Fix rolling doubles issue</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Animate tokens as gifs in GUI</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>In auction, if all bids 0, cancel auction</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Fix doubles jail issue</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Fix landing on Go issue</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sprint8!$C$3:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-15AF-4DD6-AB71-2278BE4BB518}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="456011184"/>
+        <c:axId val="456008232"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="456011184"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-CH"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="456008232"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="456008232"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="43941"/>
+          <c:min val="43934"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="t"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-CH"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="456011184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3587,6 +4019,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
   <cs:axisTitle>
@@ -6618,6 +7090,511 @@
 </file>
 
 <file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -7409,6 +8386,47 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47B3BD18-6C44-4DD8-86EA-513F308A8B03}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -8524,7 +9542,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36829F57-7CE4-479E-AFDD-4272F2EF14EF}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L35" sqref="L35"/>
     </sheetView>
   </sheetViews>
@@ -8639,11 +9657,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B97697A3-CF16-4930-B756-0AB20B140FA6}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
@@ -8661,28 +9682,70 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="2"/>
-      <c r="C3" s="5"/>
+      <c r="A3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="2">
+        <v>43934</v>
+      </c>
+      <c r="C3" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="2"/>
-      <c r="C4" s="5"/>
+      <c r="A4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="2">
+        <v>43934</v>
+      </c>
+      <c r="C4" s="5">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="2"/>
-      <c r="C5" s="5"/>
+      <c r="A5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="2">
+        <v>43934</v>
+      </c>
+      <c r="C5" s="5">
+        <v>5</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="2"/>
-      <c r="C6" s="5"/>
+      <c r="A6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" s="2">
+        <v>43935</v>
+      </c>
+      <c r="C6" s="5">
+        <v>4</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-      <c r="C7" s="5"/>
+      <c r="A7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="2">
+        <v>43936</v>
+      </c>
+      <c r="C7" s="5">
+        <v>3</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="5"/>
+      <c r="A8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" s="2">
+        <v>43939</v>
+      </c>
+      <c r="C8" s="5">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" s="2"/>
@@ -8693,10 +9756,15 @@
       <c r="C10" s="5"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:C8">
+    <sortCondition ref="B3:B8"/>
+    <sortCondition ref="C3:C8"/>
+  </sortState>
   <mergeCells count="1">
     <mergeCell ref="A1:C1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Create gantt chart for sprint 9
</commit_message>
<xml_diff>
--- a/DevelopmentDocuments/ganttCharts.xlsx
+++ b/DevelopmentDocuments/ganttCharts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agent\Desktop\Projects\PropertyTycoon\DevelopmentDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7593AC61-5882-47D6-9754-720C058C4FCF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2C26BE9-9894-4F67-8A3C-AA05E923018B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31755" yWindow="3840" windowWidth="38700" windowHeight="15885" firstSheet="3" activeTab="7" xr2:uid="{36599407-A2B4-4F4E-B01D-CD4A00EBB384}"/>
+    <workbookView xWindow="4830" yWindow="9015" windowWidth="38700" windowHeight="15885" firstSheet="3" activeTab="8" xr2:uid="{36599407-A2B4-4F4E-B01D-CD4A00EBB384}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="73">
   <si>
     <t>Sprint1</t>
   </si>
@@ -238,6 +238,27 @@
   </si>
   <si>
     <t>In auction, if all bids 0, cancel auction</t>
+  </si>
+  <si>
+    <t>Add £200 when player's loopCount increases</t>
+  </si>
+  <si>
+    <t>Implement getOutOfJailFree cards</t>
+  </si>
+  <si>
+    <t>Method to check if player can afford houses</t>
+  </si>
+  <si>
+    <t>If property owner in jail, no rent</t>
+  </si>
+  <si>
+    <t>If jailed player pays to leave, money to FreeParking</t>
+  </si>
+  <si>
+    <t>Bugs relating to last sprint</t>
+  </si>
+  <si>
+    <t>Writing documentation</t>
   </si>
 </sst>
 </file>
@@ -3684,6 +3705,432 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="456011184"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-CH"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-AU"/>
+              <a:t>Sprint 9</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-CH"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sprint9!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Start Date</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sprint9!$A$3:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>If property owner in jail, no rent</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Implement getOutOfJailFree cards</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Method to check if player can afford houses</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Bugs relating to last sprint</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Writing documentation</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Add £200 when player's loopCount increases</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>If jailed player pays to leave, money to FreeParking</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sprint9!$B$3:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>43952</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43952</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43952</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43952</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43952</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43953</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43954</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-08BB-437B-AB88-EDBCED9ACF9C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sprint9!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Duration</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sprint9!$A$3:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>If property owner in jail, no rent</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Implement getOutOfJailFree cards</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Method to check if player can afford houses</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Bugs relating to last sprint</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Writing documentation</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Add £200 when player's loopCount increases</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>If jailed player pays to leave, money to FreeParking</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sprint9!$C$3:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-08BB-437B-AB88-EDBCED9ACF9C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="445778432"/>
+        <c:axId val="699833376"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="445778432"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-CH"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="699833376"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="699833376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="43959"/>
+          <c:min val="43952"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="t"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-CH"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="445778432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4059,6 +4506,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
   <cs:axisTitle>
@@ -7595,6 +8082,511 @@
 </file>
 
 <file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -8427,6 +9419,47 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>285749</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>200024</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>42863</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F5C5E5E-41F6-4E1D-9C2B-959F69CF51EA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -9657,7 +10690,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B97697A3-CF16-4930-B756-0AB20B140FA6}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
@@ -9772,11 +10805,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F6F873B-3E4B-4741-9898-256B2E2385F0}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q41" sqref="Q41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
@@ -9794,41 +10830,95 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="2"/>
-      <c r="C3" s="5"/>
+      <c r="A3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="2">
+        <v>43952</v>
+      </c>
+      <c r="C3" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="2"/>
-      <c r="C4" s="5"/>
+      <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="2">
+        <v>43952</v>
+      </c>
+      <c r="C4" s="5">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="2"/>
-      <c r="C5" s="5"/>
+      <c r="A5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="2">
+        <v>43952</v>
+      </c>
+      <c r="C5" s="5">
+        <v>5</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="2"/>
-      <c r="C6" s="5"/>
+      <c r="A6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="2">
+        <v>43952</v>
+      </c>
+      <c r="C6" s="5">
+        <v>5</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-      <c r="C7" s="5"/>
+      <c r="A7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" s="2">
+        <v>43952</v>
+      </c>
+      <c r="C7" s="5">
+        <v>7</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="5"/>
+      <c r="A8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" s="2">
+        <v>43953</v>
+      </c>
+      <c r="C8" s="5">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B9" s="2"/>
-      <c r="C9" s="5"/>
+      <c r="A9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" s="2">
+        <v>43954</v>
+      </c>
+      <c r="C9" s="5">
+        <v>2</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" s="2"/>
       <c r="C10" s="5"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:C9">
+    <sortCondition ref="B3:B9"/>
+    <sortCondition ref="C3:C9"/>
+  </sortState>
   <mergeCells count="1">
     <mergeCell ref="A1:C1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>